<commit_message>
Baixei extençoes excel viewer dei um pip install beautifuls4
</commit_message>
<xml_diff>
--- a/data/Dados_Brasileirao.xlsx
+++ b/data/Dados_Brasileirao.xlsx
@@ -492,32 +492,32 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" t="n">
         <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" t="n">
         <v>2</v>
       </c>
       <c r="F2" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H2" t="n">
         <v>24</v>
       </c>
       <c r="I2" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>vvdvvv</t>
+          <t>vdvvve</t>
         </is>
       </c>
     </row>
@@ -528,10 +528,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="n">
         <v>4</v>
@@ -540,20 +540,20 @@
         <v>3</v>
       </c>
       <c r="F3" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G3" t="n">
         <v>11</v>
       </c>
       <c r="H3" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I3" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>evvved</t>
+          <t>vvvedv</t>
         </is>
       </c>
     </row>
@@ -564,32 +564,32 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="n">
         <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
         <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G4" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H4" t="n">
         <v>7</v>
       </c>
       <c r="I4" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>ddevvv</t>
+          <t>devvve</t>
         </is>
       </c>
     </row>
@@ -600,13 +600,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="n">
         <v>8</v>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
         <v>3</v>
@@ -621,119 +621,119 @@
         <v>7</v>
       </c>
       <c r="I5" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>dvvvev</t>
+          <t>vvveve</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5Red Bull Bragantino</t>
+          <t>5Mirassol</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G6" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I6" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>dveddd</t>
+          <t>vevvev</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>6Botafogo RJ</t>
+          <t>6Red Bull Bragantino</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C7" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
         <v>7</v>
       </c>
-      <c r="D7" t="n">
-        <v>5</v>
-      </c>
-      <c r="E7" t="n">
-        <v>3</v>
-      </c>
       <c r="F7" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G7" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="H7" t="n">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="I7" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>vvveve</t>
+          <t>vedddd</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>7Mirassol</t>
+          <t>7Botafogo RJ</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G8" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I8" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>vvevve</t>
+          <t>vveved</t>
         </is>
       </c>
     </row>
@@ -744,10 +744,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9" t="n">
         <v>7</v>
@@ -756,200 +756,200 @@
         <v>5</v>
       </c>
       <c r="F9" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G9" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H9" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>ddevvv</t>
+          <t>devvvv</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>9Ceara</t>
+          <t>9Fluminense</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>16</v>
       </c>
       <c r="C10" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
         <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G10" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="I10" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>dvdddv</t>
+          <t>vddddv</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10Internacional</t>
+          <t>10Atletico MG</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>16</v>
       </c>
       <c r="C11" t="n">
+        <v>6</v>
+      </c>
+      <c r="D11" t="n">
         <v>5</v>
-      </c>
-      <c r="D11" t="n">
-        <v>6</v>
       </c>
       <c r="E11" t="n">
         <v>5</v>
       </c>
       <c r="F11" t="n">
+        <v>18</v>
+      </c>
+      <c r="G11" t="n">
         <v>17</v>
       </c>
-      <c r="G11" t="n">
-        <v>20</v>
-      </c>
       <c r="H11" t="n">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>ddvvve</t>
+          <t>vvdddv</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>11Corinthians</t>
+          <t>11Ceara</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>17</v>
       </c>
       <c r="C12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G12" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H12" t="n">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>edvdee</t>
+          <t>vdddve</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>12Fluminense</t>
+          <t>12Corinthians</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C13" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>7</v>
+      </c>
+      <c r="E13" t="n">
         <v>6</v>
-      </c>
-      <c r="D13" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" t="n">
-        <v>7</v>
       </c>
       <c r="F13" t="n">
         <v>17</v>
       </c>
       <c r="G13" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H13" t="n">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="I13" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>vvdddd</t>
+          <t>dvdeee</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>13Atletico MG</t>
+          <t>13Internacional</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C14" t="n">
         <v>5</v>
       </c>
       <c r="D14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G14" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="I14" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>evvddd</t>
+          <t>dvvved</t>
         </is>
       </c>
     </row>
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" t="n">
         <v>5</v>
@@ -969,79 +969,79 @@
         <v>5</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
         <v>16</v>
       </c>
       <c r="G15" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H15" t="n">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="I15" t="n">
         <v>20</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>vededv</t>
+          <t>ededvd</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>15Vitoria</t>
+          <t>15Santos FC</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>17</v>
       </c>
       <c r="C16" t="n">
+        <v>5</v>
+      </c>
+      <c r="D16" t="n">
         <v>3</v>
       </c>
-      <c r="D16" t="n">
-        <v>8</v>
-      </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G16" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H16" t="n">
         <v>-4</v>
       </c>
       <c r="I16" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>edevee</t>
+          <t>vvddev</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>16Vasco da Gama</t>
+          <t>16Vitoria</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>16</v>
@@ -1053,18 +1053,18 @@
         <v>-4</v>
       </c>
       <c r="I17" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>ddvdee</t>
+          <t>deveee</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>17Santos FC</t>
+          <t>17Vasco da Gama</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1080,20 +1080,20 @@
         <v>9</v>
       </c>
       <c r="F18" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G18" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H18" t="n">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="I18" t="n">
         <v>15</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>dvvdde</t>
+          <t>dvdeed</t>
         </is>
       </c>
     </row>
@@ -1104,32 +1104,32 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" t="n">
         <v>3</v>
       </c>
       <c r="D19" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E19" t="n">
         <v>8</v>
       </c>
       <c r="F19" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G19" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H19" t="n">
         <v>-6</v>
       </c>
       <c r="I19" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>dddevd</t>
+          <t>ddevde</t>
         </is>
       </c>
     </row>
@@ -1140,7 +1140,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C20" t="n">
         <v>3</v>
@@ -1149,23 +1149,23 @@
         <v>2</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F20" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G20" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H20" t="n">
-        <v>-22</v>
+        <v>-24</v>
       </c>
       <c r="I20" t="n">
         <v>11</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>ddvddd</t>
+          <t>dvdddd</t>
         </is>
       </c>
     </row>
@@ -1176,13 +1176,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E21" t="n">
         <v>10</v>
@@ -1197,11 +1197,11 @@
         <v>-16</v>
       </c>
       <c r="I21" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>edddee</t>
+          <t>dddeee</t>
         </is>
       </c>
     </row>

</xml_diff>